<commit_message>
modifs gantt pour test et refusion
Signed-off-by: Quentin Mercier <qmercier@hotmail.fr>
</commit_message>
<xml_diff>
--- a/rapports/Gantt projet.xlsx
+++ b/rapports/Gantt projet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t xml:space="preserve">Taches </t>
   </si>
@@ -89,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -123,7 +123,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,25 +426,25 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="84443904"/>
-        <c:axId val="84445440"/>
+        <c:axId val="59107584"/>
+        <c:axId val="69996544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="84443904"/>
+        <c:axId val="59107584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84445440"/>
+        <c:crossAx val="69996544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84445440"/>
+        <c:axId val="69996544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="42030"/>
@@ -464,7 +464,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84443904"/>
+        <c:crossAx val="59107584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -478,7 +478,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -804,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1100,6 +1100,31 @@
       <c r="D19" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>